<commit_message>
found an interesting data point and almost finished the line assignment. I need help with the pkg
</commit_message>
<xml_diff>
--- a/starting with data/excel files/combined_data.xlsx
+++ b/starting with data/excel files/combined_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailtauacil-my.sharepoint.com/personal/jy1_mail_tau_ac_il/Documents/Desktop/אוניברסיטה/אסטרו נודר/פרויקט קיץ/התחלה של קוד/astro_summer_project/starting with data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailtauacil-my.sharepoint.com/personal/jy1_mail_tau_ac_il/Documents/Desktop/אוניברסיטה/אסטרו נודר/פרויקט קיץ/התחלה של קוד/astro_summer_project/starting with data/excel files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_257E863675015606E6FF31D2F8F2D3C27450C584" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DED5633D-1C98-407E-B167-3332DE57695E}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_257E863675015606E6FF31D2F8F2D3C27450C584" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{628143B1-1A39-45E2-8620-973FA3034A1F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,12 +52,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -87,11 +93,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,9 +442,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="7.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
@@ -643,17 +659,17 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="3">
         <v>0.75049745999999995</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="3">
         <v>18.34</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <v>0.08</v>
       </c>
     </row>

</xml_diff>

<commit_message>
this is it, making the new model. my temp function is not working. i'll check it timmorow
</commit_message>
<xml_diff>
--- a/starting with data/excel files/combined_data.xlsx
+++ b/starting with data/excel files/combined_data.xlsx
@@ -8,19 +8,47 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailtauacil-my.sharepoint.com/personal/jy1_mail_tau_ac_il/Documents/Desktop/אוניברסיטה/אסטרו נודר/פרויקט קיץ/התחלה של קוד/astro_summer_project/starting with data/excel files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_257E863675015606E6FF31D2F8F2D3C27450C584" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{628143B1-1A39-45E2-8620-973FA3034A1F}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="11_257E863675015606E6FF31D2F8F2D3C27450C584" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C933D923-85A9-4736-B674-4B6C7DAA8F10}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rel data for graph" sheetId="1" r:id="rId1"/>
+    <sheet name="after extinction" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={3166CBF0-8F73-4AC9-9524-116742E9495F}</author>
+    <author>tc={704B4418-2CD3-450F-8DA9-78DC0A883B00}</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{3166CBF0-8F73-4AC9-9524-116742E9495F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    i took of 0.052 for the extinction</t>
+      </text>
+    </comment>
+    <comment ref="C73" authorId="1" shapeId="0" xr:uid="{704B4418-2CD3-450F-8DA9-78DC0A883B00}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    כאן הנתונים שלהם מסתיימים</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>JD - 2457651.0[day]</t>
   </si>
@@ -35,7 +63,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,6 +78,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -93,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -102,6 +136,8 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -117,6 +153,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Jonathan Yerushalmi" id="{2B0FD18F-B902-4BC1-8991-44E47D4C0435}" userId="S::jy1@mail.tau.ac.il::cc673c71-658d-4b15-9c0d-2ac25539ec95" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -438,11 +480,22 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B2" dT="2022-08-31T13:24:42.55" personId="{2B0FD18F-B902-4BC1-8991-44E47D4C0435}" id="{3166CBF0-8F73-4AC9-9524-116742E9495F}">
+    <text>i took of 0.052 for the extinction</text>
+  </threadedComment>
+  <threadedComment ref="C73" dT="2022-08-31T13:33:01.60" personId="{2B0FD18F-B902-4BC1-8991-44E47D4C0435}" id="{704B4418-2CD3-450F-8DA9-78DC0A883B00}">
+    <text>כאן הנתונים שלהם מסתיימים</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -1362,4 +1415,1349 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E908E7-5368-407B-A5EC-78B3D29B445E}">
+  <dimension ref="A1:C121"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>0.7361548</v>
+      </c>
+      <c r="B2" s="4">
+        <v>18.977</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>0.73452949000000001</v>
+      </c>
+      <c r="B3" s="4">
+        <v>19.056999999999999</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>0.73629635999999998</v>
+      </c>
+      <c r="B4" s="4">
+        <v>18.966999999999999</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>0.73793518000000002</v>
+      </c>
+      <c r="B5" s="4">
+        <v>18.927</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>0.73376156999999997</v>
+      </c>
+      <c r="B6" s="4">
+        <v>18.896999999999998</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>0.73410880000000001</v>
+      </c>
+      <c r="B7" s="4">
+        <v>19.497</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>0.73439814999999997</v>
+      </c>
+      <c r="B8" s="4">
+        <v>18.896999999999998</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>0.73468750000000005</v>
+      </c>
+      <c r="B9" s="4">
+        <v>18.716999999999999</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>0.73496528000000005</v>
+      </c>
+      <c r="B10" s="4">
+        <v>19.596999999999998</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>0.73525463000000002</v>
+      </c>
+      <c r="B11" s="4">
+        <v>19.356999999999999</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>0.73554397999999999</v>
+      </c>
+      <c r="B12" s="4">
+        <v>18.957000000000001</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>0.73585648000000003</v>
+      </c>
+      <c r="B13" s="4">
+        <v>19.207000000000001</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>0.73614583</v>
+      </c>
+      <c r="B14" s="4">
+        <v>19.087</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>0.73644675999999998</v>
+      </c>
+      <c r="B15" s="4">
+        <v>18.396999999999998</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>0.73673611000000006</v>
+      </c>
+      <c r="B16" s="4">
+        <v>19.346999999999998</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>0.73704860999999999</v>
+      </c>
+      <c r="B17" s="4">
+        <v>19.536999999999999</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>0.73734953999999997</v>
+      </c>
+      <c r="B18" s="4">
+        <v>19.117000000000001</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>0.73765046000000001</v>
+      </c>
+      <c r="B19" s="4">
+        <v>19.177</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>0.73793982000000002</v>
+      </c>
+      <c r="B20" s="4">
+        <v>18.617000000000001</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>0.73822916999999999</v>
+      </c>
+      <c r="B21" s="4">
+        <v>18.966999999999999</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>0.73850693999999995</v>
+      </c>
+      <c r="B22" s="4">
+        <v>18.846999999999998</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>0.74201744999999997</v>
+      </c>
+      <c r="B23" s="4">
+        <v>18.766999999999999</v>
+      </c>
+      <c r="C23" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>0.73999994999999996</v>
+      </c>
+      <c r="B24" s="4">
+        <v>18.696999999999999</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>0.74130099999999999</v>
+      </c>
+      <c r="B25" s="4">
+        <v>18.696999999999999</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>0.74262035000000004</v>
+      </c>
+      <c r="B26" s="4">
+        <v>18.736999999999998</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>0.74414860999999999</v>
+      </c>
+      <c r="B27" s="4">
+        <v>18.736999999999998</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>0.73947916999999996</v>
+      </c>
+      <c r="B28" s="4">
+        <v>18.536999999999999</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>0.73974536999999996</v>
+      </c>
+      <c r="B29" s="4">
+        <v>18.876999999999999</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>0.74</v>
+      </c>
+      <c r="B30" s="4">
+        <v>18.766999999999999</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>0.74025463000000002</v>
+      </c>
+      <c r="B31" s="4">
+        <v>19.146999999999998</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>0.74052083000000002</v>
+      </c>
+      <c r="B32" s="4">
+        <v>18.477</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>0.74077546000000005</v>
+      </c>
+      <c r="B33" s="4">
+        <v>18.997</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>0.74104166999999999</v>
+      </c>
+      <c r="B34" s="4">
+        <v>18.297000000000001</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>0.74129630000000002</v>
+      </c>
+      <c r="B35" s="4">
+        <v>18.957000000000001</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>0.74156250000000001</v>
+      </c>
+      <c r="B36" s="4">
+        <v>18.466999999999999</v>
+      </c>
+      <c r="C36" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>0.74182870000000001</v>
+      </c>
+      <c r="B37" s="4">
+        <v>18.986999999999998</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>0.74208333000000004</v>
+      </c>
+      <c r="B38" s="4">
+        <v>18.407</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>0.74234953999999997</v>
+      </c>
+      <c r="B39" s="4">
+        <v>19.826999999999998</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>0.74261573999999997</v>
+      </c>
+      <c r="B40" s="4">
+        <v>19.266999999999999</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>0.74287037</v>
+      </c>
+      <c r="B41" s="4">
+        <v>18.657</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>0.74318287000000005</v>
+      </c>
+      <c r="B42" s="4">
+        <v>18.776999999999997</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>0.74351851999999996</v>
+      </c>
+      <c r="B43" s="4">
+        <v>18.887</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>0.74384258999999997</v>
+      </c>
+      <c r="B44" s="4">
+        <v>18.957000000000001</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>0.74414351999999995</v>
+      </c>
+      <c r="B45" s="4">
+        <v>18.986999999999998</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>0.74446758999999996</v>
+      </c>
+      <c r="B46" s="4">
+        <v>18.576999999999998</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>0.74476852000000004</v>
+      </c>
+      <c r="B47" s="4">
+        <v>18.526999999999997</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>0.74817347000000001</v>
+      </c>
+      <c r="B48" s="4">
+        <v>18.427</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>0.74595498999999998</v>
+      </c>
+      <c r="B49" s="4">
+        <v>18.407</v>
+      </c>
+      <c r="C49" s="4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>0.74763661999999997</v>
+      </c>
+      <c r="B50" s="4">
+        <v>18.547000000000001</v>
+      </c>
+      <c r="C50" s="4">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>0.74904883</v>
+      </c>
+      <c r="B51" s="4">
+        <v>18.497</v>
+      </c>
+      <c r="C51" s="4">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>0.75049745999999995</v>
+      </c>
+      <c r="B52" s="4">
+        <v>18.286999999999999</v>
+      </c>
+      <c r="C52" s="4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>0.74512730999999999</v>
+      </c>
+      <c r="B53" s="4">
+        <v>18.646999999999998</v>
+      </c>
+      <c r="C53" s="4">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>0.74550925999999995</v>
+      </c>
+      <c r="B54" s="4">
+        <v>18.337</v>
+      </c>
+      <c r="C54" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>0.74582176</v>
+      </c>
+      <c r="B55" s="4">
+        <v>18.747</v>
+      </c>
+      <c r="C55" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>0.74612268999999998</v>
+      </c>
+      <c r="B56" s="4">
+        <v>18.707000000000001</v>
+      </c>
+      <c r="C56" s="4">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>0.74642361000000002</v>
+      </c>
+      <c r="B57" s="4">
+        <v>18.056999999999999</v>
+      </c>
+      <c r="C57" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>0.74672453999999999</v>
+      </c>
+      <c r="B58" s="4">
+        <v>18.416999999999998</v>
+      </c>
+      <c r="C58" s="4">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>0.74706019000000001</v>
+      </c>
+      <c r="B59" s="4">
+        <v>18.376999999999999</v>
+      </c>
+      <c r="C59" s="4">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <v>0.74737268999999995</v>
+      </c>
+      <c r="B60" s="4">
+        <v>18.617000000000001</v>
+      </c>
+      <c r="C60" s="4">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
+        <v>0.74765046000000002</v>
+      </c>
+      <c r="B61" s="4">
+        <v>18.786999999999999</v>
+      </c>
+      <c r="C61" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
+        <v>0.74791666999999995</v>
+      </c>
+      <c r="B62" s="4">
+        <v>18.497</v>
+      </c>
+      <c r="C62" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="4">
+        <v>0.74818287000000006</v>
+      </c>
+      <c r="B63" s="4">
+        <v>18.376999999999999</v>
+      </c>
+      <c r="C63" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="4">
+        <v>0.74843749999999998</v>
+      </c>
+      <c r="B64" s="4">
+        <v>18.576999999999998</v>
+      </c>
+      <c r="C64" s="4">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="4">
+        <v>0.74870369999999997</v>
+      </c>
+      <c r="B65" s="4">
+        <v>18.297000000000001</v>
+      </c>
+      <c r="C65" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
+        <v>0.74906249999999996</v>
+      </c>
+      <c r="B66" s="4">
+        <v>18.567</v>
+      </c>
+      <c r="C66" s="4">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="4">
+        <v>0.74938656999999997</v>
+      </c>
+      <c r="B67" s="4">
+        <v>18.137</v>
+      </c>
+      <c r="C67" s="4">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
+        <v>0.74965278000000002</v>
+      </c>
+      <c r="B68" s="4">
+        <v>19.117000000000001</v>
+      </c>
+      <c r="C68" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
+        <v>0.74994212999999998</v>
+      </c>
+      <c r="B69" s="4">
+        <v>18.256999999999998</v>
+      </c>
+      <c r="C69" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
+        <v>0.75023147999999995</v>
+      </c>
+      <c r="B70" s="4">
+        <v>18.376999999999999</v>
+      </c>
+      <c r="C70" s="4">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="4">
+        <v>0.75050925999999996</v>
+      </c>
+      <c r="B71" s="4">
+        <v>18.177</v>
+      </c>
+      <c r="C71" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="4">
+        <v>0.75077545999999995</v>
+      </c>
+      <c r="B72" s="4">
+        <v>18.457000000000001</v>
+      </c>
+      <c r="C72" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="5">
+        <v>0.75103008999999998</v>
+      </c>
+      <c r="B73" s="5">
+        <v>18.266999999999999</v>
+      </c>
+      <c r="C73" s="5">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>1.799000000115484</v>
+      </c>
+      <c r="B74" s="4">
+        <v>14.672000000000001</v>
+      </c>
+      <c r="C74" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
+        <v>1.799000000115484</v>
+      </c>
+      <c r="B75" s="4">
+        <v>14.672000000000001</v>
+      </c>
+      <c r="C75" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
+        <v>2.1650000000372529</v>
+      </c>
+      <c r="B76" s="4">
+        <v>14.789</v>
+      </c>
+      <c r="C76" s="4">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="4">
+        <v>2.2310000001452859</v>
+      </c>
+      <c r="B77" s="4">
+        <v>14.957000000000001</v>
+      </c>
+      <c r="C77" s="4">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="4">
+        <v>2.6069999998435378</v>
+      </c>
+      <c r="B78" s="4">
+        <v>15.106</v>
+      </c>
+      <c r="C78" s="4">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="4">
+        <v>2.608000000007451</v>
+      </c>
+      <c r="B79" s="4">
+        <v>15.102</v>
+      </c>
+      <c r="C79" s="4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="4">
+        <v>2.6290000001899898</v>
+      </c>
+      <c r="B80" s="4">
+        <v>15.202</v>
+      </c>
+      <c r="C80" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="4">
+        <v>2.6290000001899898</v>
+      </c>
+      <c r="B81" s="4">
+        <v>15.202</v>
+      </c>
+      <c r="C81" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="4">
+        <v>2.7880000001750891</v>
+      </c>
+      <c r="B82" s="4">
+        <v>15.391999999999999</v>
+      </c>
+      <c r="C82" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="4">
+        <v>2.7880000001750891</v>
+      </c>
+      <c r="B83" s="4">
+        <v>15.391999999999999</v>
+      </c>
+      <c r="C83" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="4">
+        <v>2.8209999999962752</v>
+      </c>
+      <c r="B84" s="4">
+        <v>15.273999999999999</v>
+      </c>
+      <c r="C84" s="4">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
+        <v>2.822000000160187</v>
+      </c>
+      <c r="B85" s="4">
+        <v>15.247</v>
+      </c>
+      <c r="C85" s="4">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="4">
+        <v>2.8960000001825388</v>
+      </c>
+      <c r="B86" s="4">
+        <v>15.502000000000001</v>
+      </c>
+      <c r="C86" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="4">
+        <v>2.8960000001825388</v>
+      </c>
+      <c r="B87" s="4">
+        <v>15.502000000000001</v>
+      </c>
+      <c r="C87" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="4">
+        <v>3.2349999998696148</v>
+      </c>
+      <c r="B88" s="4">
+        <v>15.651999999999999</v>
+      </c>
+      <c r="C88" s="4">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="4">
+        <v>3.31900000013411</v>
+      </c>
+      <c r="B89" s="4">
+        <v>15.756</v>
+      </c>
+      <c r="C89" s="4">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="4">
+        <v>3.3199999998323619</v>
+      </c>
+      <c r="B90" s="4">
+        <v>15.949</v>
+      </c>
+      <c r="C90" s="4">
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="4">
+        <v>3.572999999858439</v>
+      </c>
+      <c r="B91" s="4">
+        <v>16.023</v>
+      </c>
+      <c r="C91" s="4">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="4">
+        <v>3.5740000000223522</v>
+      </c>
+      <c r="B92" s="4">
+        <v>16.044</v>
+      </c>
+      <c r="C92" s="4">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="4">
+        <v>3.6669999998994172</v>
+      </c>
+      <c r="B93" s="4">
+        <v>16.059000000000001</v>
+      </c>
+      <c r="C93" s="4">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="4">
+        <v>3.6680000000633299</v>
+      </c>
+      <c r="B94" s="4">
+        <v>16.085000000000001</v>
+      </c>
+      <c r="C94" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="4">
+        <v>3.697999999858439</v>
+      </c>
+      <c r="B95" s="4">
+        <v>16.114999999999998</v>
+      </c>
+      <c r="C95" s="4">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="4">
+        <v>3.6990000000223522</v>
+      </c>
+      <c r="B96" s="4">
+        <v>16.123000000000001</v>
+      </c>
+      <c r="C96" s="4">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="4">
+        <v>3.8739999998360868</v>
+      </c>
+      <c r="B97" s="4">
+        <v>16.207999999999998</v>
+      </c>
+      <c r="C97" s="4">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="4">
+        <v>3.875</v>
+      </c>
+      <c r="B98" s="4">
+        <v>16.187000000000001</v>
+      </c>
+      <c r="C98" s="4">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="4">
+        <v>3.8879999998025601</v>
+      </c>
+      <c r="B99" s="4">
+        <v>16.282</v>
+      </c>
+      <c r="C99" s="4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="4">
+        <v>3.8889999999664719</v>
+      </c>
+      <c r="B100" s="4">
+        <v>16.289000000000001</v>
+      </c>
+      <c r="C100" s="4">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="4">
+        <v>4.3209999999962747</v>
+      </c>
+      <c r="B101" s="4">
+        <v>16.234999999999999</v>
+      </c>
+      <c r="C101" s="4">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="4">
+        <v>4.3220000001601866</v>
+      </c>
+      <c r="B102" s="4">
+        <v>16.344999999999999</v>
+      </c>
+      <c r="C102" s="4">
+        <v>3.1E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="4">
+        <v>4.6889999997802079</v>
+      </c>
+      <c r="B103" s="4">
+        <v>16.372</v>
+      </c>
+      <c r="C103" s="4">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="4">
+        <v>4.6899999999441206</v>
+      </c>
+      <c r="B104" s="4">
+        <v>16.323</v>
+      </c>
+      <c r="C104" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="4">
+        <v>4.7289999998174608</v>
+      </c>
+      <c r="B105" s="4">
+        <v>16.318999999999999</v>
+      </c>
+      <c r="C105" s="4">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="4">
+        <v>4.7299999999813744</v>
+      </c>
+      <c r="B106" s="4">
+        <v>16.29</v>
+      </c>
+      <c r="C106" s="4">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="4">
+        <v>5.3130000000819564</v>
+      </c>
+      <c r="B107" s="4">
+        <v>16.155999999999999</v>
+      </c>
+      <c r="C107" s="4">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="4">
+        <v>5.3139999997802079</v>
+      </c>
+      <c r="B108" s="4">
+        <v>16.265000000000001</v>
+      </c>
+      <c r="C108" s="4">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="4">
+        <v>5.4589999997988343</v>
+      </c>
+      <c r="B109" s="4">
+        <v>16.111000000000001</v>
+      </c>
+      <c r="C109" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="4">
+        <v>5.4599999999627471</v>
+      </c>
+      <c r="B110" s="4">
+        <v>16.131</v>
+      </c>
+      <c r="C110" s="4">
+        <v>4.1000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="4">
+        <v>5.5180000001564622</v>
+      </c>
+      <c r="B111" s="4">
+        <v>16.140999999999998</v>
+      </c>
+      <c r="C111" s="4">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="4">
+        <v>5.5189999998547137</v>
+      </c>
+      <c r="B112" s="4">
+        <v>16.184999999999999</v>
+      </c>
+      <c r="C112" s="4">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="4">
+        <v>5.546000000089407</v>
+      </c>
+      <c r="B113" s="4">
+        <v>16.196999999999999</v>
+      </c>
+      <c r="C113" s="4">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="4">
+        <v>5.5469999997876576</v>
+      </c>
+      <c r="B114" s="4">
+        <v>16.224</v>
+      </c>
+      <c r="C114" s="4">
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="4">
+        <v>6.4160000002011657</v>
+      </c>
+      <c r="B115" s="4">
+        <v>15.949</v>
+      </c>
+      <c r="C115" s="4">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="4">
+        <v>6.4180000000633299</v>
+      </c>
+      <c r="B116" s="4">
+        <v>15.935</v>
+      </c>
+      <c r="C116" s="4">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="4">
+        <v>6.5049999998882413</v>
+      </c>
+      <c r="B117" s="4">
+        <v>15.881</v>
+      </c>
+      <c r="C117" s="4">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="4">
+        <v>6.5060000000521541</v>
+      </c>
+      <c r="B118" s="4">
+        <v>15.925000000000001</v>
+      </c>
+      <c r="C118" s="4">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="4">
+        <v>6.5800000000745058</v>
+      </c>
+      <c r="B119" s="4">
+        <v>15.965</v>
+      </c>
+      <c r="C119" s="4">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="4">
+        <v>6.5849999999627471</v>
+      </c>
+      <c r="B120" s="4">
+        <v>15.837</v>
+      </c>
+      <c r="C120" s="4">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="4">
+        <v>6.5860000001266599</v>
+      </c>
+      <c r="B121" s="4">
+        <v>15.906000000000001</v>
+      </c>
+      <c r="C121" s="4">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
made it, need to learn about the server
</commit_message>
<xml_diff>
--- a/starting with data/excel files/combined_data.xlsx
+++ b/starting with data/excel files/combined_data.xlsx
@@ -8,15 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailtauacil-my.sharepoint.com/personal/jy1_mail_tau_ac_il/Documents/Desktop/אוניברסיטה/אסטרו נודר/פרויקט קיץ/התחלה של קוד/astro_summer_project/starting with data/excel files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_257E863675015606E6FF31D2F8F2D3C27450C584" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C933D923-85A9-4736-B674-4B6C7DAA8F10}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="11_257E863675015606E6FF31D2F8F2D3C27450C584" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D14DB0E3-FF4D-4054-9BCB-0E00140DAE26}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rel data for graph" sheetId="1" r:id="rId1"/>
     <sheet name="after extinction" sheetId="2" r:id="rId2"/>
+    <sheet name="after ext binning" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -47,8 +61,26 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={964449A5-0BC3-4EBA-BD37-697AAB2DEFEB}</author>
+  </authors>
+  <commentList>
+    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{964449A5-0BC3-4EBA-BD37-697AAB2DEFEB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    the end of their data</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
   <si>
     <t>JD - 2457651.0[day]</t>
   </si>
@@ -63,7 +95,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,14 +111,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,6 +122,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -127,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -138,6 +170,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,6 +525,14 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A15" dT="2022-09-04T07:02:34.91" personId="{2B0FD18F-B902-4BC1-8991-44E47D4C0435}" id="{964449A5-0BC3-4EBA-BD37-697AAB2DEFEB}">
+    <text>the end of their data</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D65"/>
@@ -1421,7 +1463,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E908E7-5368-407B-A5EC-78B3D29B445E}">
   <dimension ref="A1:C121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:C121"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2760,4 +2804,587 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D05F4C15-D03C-490A-AF28-C979BDCD01FF}">
+  <dimension ref="A1:C63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>0.7361548</v>
+      </c>
+      <c r="B2" s="4">
+        <v>18.978000000000002</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>0.73452949000000001</v>
+      </c>
+      <c r="B3" s="4">
+        <v>19.058</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>0.73629635999999998</v>
+      </c>
+      <c r="B4" s="4">
+        <v>18.968</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>0.73793518000000002</v>
+      </c>
+      <c r="B5" s="4">
+        <v>18.928000000000001</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>0.74201744999999997</v>
+      </c>
+      <c r="B6" s="4">
+        <v>18.768000000000001</v>
+      </c>
+      <c r="C6" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>0.73999994999999996</v>
+      </c>
+      <c r="B7" s="4">
+        <v>18.698</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>0.74130099999999999</v>
+      </c>
+      <c r="B8" s="4">
+        <v>18.698</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>0.74262035000000004</v>
+      </c>
+      <c r="B9" s="4">
+        <v>18.738</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>0.74414860999999999</v>
+      </c>
+      <c r="B10" s="4">
+        <v>18.738</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>0.74817347000000001</v>
+      </c>
+      <c r="B11" s="4">
+        <v>18.428000000000001</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>0.74595498999999998</v>
+      </c>
+      <c r="B12" s="4">
+        <v>18.408000000000001</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>0.74763661999999997</v>
+      </c>
+      <c r="B13" s="4">
+        <v>18.548000000000002</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>0.74904883</v>
+      </c>
+      <c r="B14" s="4">
+        <v>18.498000000000001</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>0.75049745999999995</v>
+      </c>
+      <c r="B15" s="6">
+        <v>18.288</v>
+      </c>
+      <c r="C15" s="6">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>1.799000000115484</v>
+      </c>
+      <c r="B16" s="4">
+        <v>14.672000000000001</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>1.799000000115484</v>
+      </c>
+      <c r="B17" s="4">
+        <v>14.672000000000001</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>2.1650000000372529</v>
+      </c>
+      <c r="B18" s="4">
+        <v>14.789</v>
+      </c>
+      <c r="C18" s="4">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>2.2310000001452859</v>
+      </c>
+      <c r="B19" s="4">
+        <v>14.957000000000001</v>
+      </c>
+      <c r="C19" s="4">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>2.6069999998435378</v>
+      </c>
+      <c r="B20" s="4">
+        <v>15.106</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>2.608000000007451</v>
+      </c>
+      <c r="B21" s="4">
+        <v>15.102</v>
+      </c>
+      <c r="C21" s="4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>2.6290000001899898</v>
+      </c>
+      <c r="B22" s="4">
+        <v>15.202</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>2.6290000001899898</v>
+      </c>
+      <c r="B23" s="4">
+        <v>15.202</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>2.7880000001750891</v>
+      </c>
+      <c r="B24" s="4">
+        <v>15.391999999999999</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>2.7880000001750891</v>
+      </c>
+      <c r="B25" s="4">
+        <v>15.391999999999999</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>2.8209999999962752</v>
+      </c>
+      <c r="B26" s="4">
+        <v>15.273999999999999</v>
+      </c>
+      <c r="C26" s="4">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>2.822000000160187</v>
+      </c>
+      <c r="B27" s="4">
+        <v>15.247</v>
+      </c>
+      <c r="C27" s="4">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>2.8960000001825388</v>
+      </c>
+      <c r="B28" s="4">
+        <v>15.502000000000001</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>2.8960000001825388</v>
+      </c>
+      <c r="B29" s="4">
+        <v>15.502000000000001</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>3.2349999998696148</v>
+      </c>
+      <c r="B30" s="4">
+        <v>15.651999999999999</v>
+      </c>
+      <c r="C30" s="4">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>3.31900000013411</v>
+      </c>
+      <c r="B31" s="4">
+        <v>15.756</v>
+      </c>
+      <c r="C31" s="4">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>3.3199999998323619</v>
+      </c>
+      <c r="B32" s="4">
+        <v>15.949</v>
+      </c>
+      <c r="C32" s="4">
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>3.572999999858439</v>
+      </c>
+      <c r="B33" s="4">
+        <v>16.023</v>
+      </c>
+      <c r="C33" s="4">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>3.5740000000223522</v>
+      </c>
+      <c r="B34" s="4">
+        <v>16.044</v>
+      </c>
+      <c r="C34" s="4">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>3.6669999998994172</v>
+      </c>
+      <c r="B35" s="4">
+        <v>16.059000000000001</v>
+      </c>
+      <c r="C35" s="4">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>3.6680000000633299</v>
+      </c>
+      <c r="B36" s="4">
+        <v>16.085000000000001</v>
+      </c>
+      <c r="C36" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>3.697999999858439</v>
+      </c>
+      <c r="B37" s="4">
+        <v>16.114999999999998</v>
+      </c>
+      <c r="C37" s="4">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>3.6990000000223522</v>
+      </c>
+      <c r="B38" s="4">
+        <v>16.123000000000001</v>
+      </c>
+      <c r="C38" s="4">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>3.8739999998360868</v>
+      </c>
+      <c r="B39" s="4">
+        <v>16.207999999999998</v>
+      </c>
+      <c r="C39" s="4">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>3.875</v>
+      </c>
+      <c r="B40" s="4">
+        <v>16.187000000000001</v>
+      </c>
+      <c r="C40" s="4">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>3.8879999998025601</v>
+      </c>
+      <c r="B41" s="4">
+        <v>16.282</v>
+      </c>
+      <c r="C41" s="4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>3.8889999999664719</v>
+      </c>
+      <c r="B42" s="4">
+        <v>16.289000000000001</v>
+      </c>
+      <c r="C42" s="4">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="7"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="7"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="7"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="7"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="7"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="7"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
well, it's probably not the case after all, but i gave it one last try
</commit_message>
<xml_diff>
--- a/starting with data/excel files/combined_data.xlsx
+++ b/starting with data/excel files/combined_data.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailtauacil-my.sharepoint.com/personal/jy1_mail_tau_ac_il/Documents/Desktop/אוניברסיטה/אסטרו נודר/פרויקט קיץ/התחלה של קוד/astro_summer_project/starting with data/excel files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="11_257E863675015606E6FF31D2F8F2D3C27450C584" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D14DB0E3-FF4D-4054-9BCB-0E00140DAE26}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="11_257E863675015606E6FF31D2F8F2D3C27450C584" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3003E06-C118-4325-B85E-725A708DC5D1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rel data for graph" sheetId="1" r:id="rId1"/>
-    <sheet name="after extinction" sheetId="2" r:id="rId2"/>
+    <sheet name="after ext all" sheetId="2" r:id="rId2"/>
     <sheet name="after ext binning" sheetId="3" r:id="rId3"/>
+    <sheet name="after ext" sheetId="4" r:id="rId4"/>
+    <sheet name="after ext weighted" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,10 +66,19 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={9242D3A2-D8DE-47EC-BA1A-64A3279CEC1A}</author>
     <author>tc={964449A5-0BC3-4EBA-BD37-697AAB2DEFEB}</author>
   </authors>
   <commentList>
-    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{964449A5-0BC3-4EBA-BD37-697AAB2DEFEB}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{9242D3A2-D8DE-47EC-BA1A-64A3279CEC1A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    only the binning data, and our data</t>
+      </text>
+    </comment>
+    <comment ref="A15" authorId="1" shapeId="0" xr:uid="{964449A5-0BC3-4EBA-BD37-697AAB2DEFEB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -79,8 +90,80 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={4624C9B1-6880-4992-84E6-7A676D025B27}</author>
+    <author>tc={E0831A59-86C9-4839-B97B-1ADC7DE4A368}</author>
+    <author>tc={A457C759-3D2F-4E9B-B6DC-BE9CCE413303}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{4624C9B1-6880-4992-84E6-7A676D025B27}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    all thier data and our data</t>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="1" shapeId="0" xr:uid="{E0831A59-86C9-4839-B97B-1ADC7DE4A368}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    i took of 0.052 for the extinction</t>
+      </text>
+    </comment>
+    <comment ref="C73" authorId="2" shapeId="0" xr:uid="{A457C759-3D2F-4E9B-B6DC-BE9CCE413303}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    כאן הנתונים שלהם מסתיימים</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={A3692A04-8888-4AC8-AB95-764739EFA998}</author>
+    <author>tc={073DCDB3-83CA-4E6B-851F-AF28736616E1}</author>
+    <author>tc={DB919E73-47E9-42A8-A10F-72F94CA9B858}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{A3692A04-8888-4AC8-AB95-764739EFA998}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    all thier data and our data wieghted so that every point apears twice</t>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="1" shapeId="0" xr:uid="{073DCDB3-83CA-4E6B-851F-AF28736616E1}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    i took of 0.052 for the extinction</t>
+      </text>
+    </comment>
+    <comment ref="C73" authorId="2" shapeId="0" xr:uid="{DB919E73-47E9-42A8-A10F-72F94CA9B858}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    כאן הנתונים שלהם מסתיימים</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="3">
   <si>
     <t>JD - 2457651.0[day]</t>
   </si>
@@ -95,7 +178,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +193,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="177"/>
     </font>
   </fonts>
   <fills count="4">
@@ -527,8 +616,39 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2022-09-05T12:58:17.65" personId="{2B0FD18F-B902-4BC1-8991-44E47D4C0435}" id="{9242D3A2-D8DE-47EC-BA1A-64A3279CEC1A}">
+    <text>only the binning data, and our data</text>
+  </threadedComment>
   <threadedComment ref="A15" dT="2022-09-04T07:02:34.91" personId="{2B0FD18F-B902-4BC1-8991-44E47D4C0435}" id="{964449A5-0BC3-4EBA-BD37-697AAB2DEFEB}">
     <text>the end of their data</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2022-09-05T12:58:37.70" personId="{2B0FD18F-B902-4BC1-8991-44E47D4C0435}" id="{4624C9B1-6880-4992-84E6-7A676D025B27}">
+    <text>all thier data and our data</text>
+  </threadedComment>
+  <threadedComment ref="B2" dT="2022-08-31T13:24:42.55" personId="{2B0FD18F-B902-4BC1-8991-44E47D4C0435}" id="{E0831A59-86C9-4839-B97B-1ADC7DE4A368}">
+    <text>i took of 0.052 for the extinction</text>
+  </threadedComment>
+  <threadedComment ref="C73" dT="2022-08-31T13:33:01.60" personId="{2B0FD18F-B902-4BC1-8991-44E47D4C0435}" id="{A457C759-3D2F-4E9B-B6DC-BE9CCE413303}">
+    <text>כאן הנתונים שלהם מסתיימים</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2022-09-05T12:58:37.70" personId="{2B0FD18F-B902-4BC1-8991-44E47D4C0435}" id="{A3692A04-8888-4AC8-AB95-764739EFA998}">
+    <text>all thier data and our data wieghted so that every point apears twice</text>
+  </threadedComment>
+  <threadedComment ref="B2" dT="2022-08-31T13:24:42.55" personId="{2B0FD18F-B902-4BC1-8991-44E47D4C0435}" id="{073DCDB3-83CA-4E6B-851F-AF28736616E1}">
+    <text>i took of 0.052 for the extinction</text>
+  </threadedComment>
+  <threadedComment ref="C73" dT="2022-08-31T13:33:01.60" personId="{2B0FD18F-B902-4BC1-8991-44E47D4C0435}" id="{DB919E73-47E9-42A8-A10F-72F94CA9B858}">
+    <text>כאן הנתונים שלהם מסתיימים</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -1463,8 +1583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E908E7-5368-407B-A5EC-78B3D29B445E}">
   <dimension ref="A1:C121"/>
   <sheetViews>
-    <sheetView topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74:C121"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2810,8 +2930,589 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D05F4C15-D03C-490A-AF28-C979BDCD01FF}">
   <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>0.7361548</v>
+      </c>
+      <c r="B2" s="4">
+        <v>18.978000000000002</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>0.73452949000000001</v>
+      </c>
+      <c r="B3" s="4">
+        <v>19.058</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>0.73629635999999998</v>
+      </c>
+      <c r="B4" s="4">
+        <v>18.968</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>0.73793518000000002</v>
+      </c>
+      <c r="B5" s="4">
+        <v>18.928000000000001</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>0.74201744999999997</v>
+      </c>
+      <c r="B6" s="4">
+        <v>18.768000000000001</v>
+      </c>
+      <c r="C6" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>0.73999994999999996</v>
+      </c>
+      <c r="B7" s="4">
+        <v>18.698</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>0.74130099999999999</v>
+      </c>
+      <c r="B8" s="4">
+        <v>18.698</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>0.74262035000000004</v>
+      </c>
+      <c r="B9" s="4">
+        <v>18.738</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>0.74414860999999999</v>
+      </c>
+      <c r="B10" s="4">
+        <v>18.738</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>0.74817347000000001</v>
+      </c>
+      <c r="B11" s="4">
+        <v>18.428000000000001</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>0.74595498999999998</v>
+      </c>
+      <c r="B12" s="4">
+        <v>18.408000000000001</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>0.74763661999999997</v>
+      </c>
+      <c r="B13" s="4">
+        <v>18.548000000000002</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>0.74904883</v>
+      </c>
+      <c r="B14" s="4">
+        <v>18.498000000000001</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>0.75049745999999995</v>
+      </c>
+      <c r="B15" s="6">
+        <v>18.288</v>
+      </c>
+      <c r="C15" s="6">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>1.799000000115484</v>
+      </c>
+      <c r="B16" s="4">
+        <v>14.672000000000001</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>1.799000000115484</v>
+      </c>
+      <c r="B17" s="4">
+        <v>14.672000000000001</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>2.1650000000372529</v>
+      </c>
+      <c r="B18" s="4">
+        <v>14.789</v>
+      </c>
+      <c r="C18" s="4">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>2.2310000001452859</v>
+      </c>
+      <c r="B19" s="4">
+        <v>14.957000000000001</v>
+      </c>
+      <c r="C19" s="4">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>2.6069999998435378</v>
+      </c>
+      <c r="B20" s="4">
+        <v>15.106</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>2.608000000007451</v>
+      </c>
+      <c r="B21" s="4">
+        <v>15.102</v>
+      </c>
+      <c r="C21" s="4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>2.6290000001899898</v>
+      </c>
+      <c r="B22" s="4">
+        <v>15.202</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>2.6290000001899898</v>
+      </c>
+      <c r="B23" s="4">
+        <v>15.202</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>2.7880000001750891</v>
+      </c>
+      <c r="B24" s="4">
+        <v>15.391999999999999</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>2.7880000001750891</v>
+      </c>
+      <c r="B25" s="4">
+        <v>15.391999999999999</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>2.8209999999962752</v>
+      </c>
+      <c r="B26" s="4">
+        <v>15.273999999999999</v>
+      </c>
+      <c r="C26" s="4">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>2.822000000160187</v>
+      </c>
+      <c r="B27" s="4">
+        <v>15.247</v>
+      </c>
+      <c r="C27" s="4">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>2.8960000001825388</v>
+      </c>
+      <c r="B28" s="4">
+        <v>15.502000000000001</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>2.8960000001825388</v>
+      </c>
+      <c r="B29" s="4">
+        <v>15.502000000000001</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>3.2349999998696148</v>
+      </c>
+      <c r="B30" s="4">
+        <v>15.651999999999999</v>
+      </c>
+      <c r="C30" s="4">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>3.31900000013411</v>
+      </c>
+      <c r="B31" s="4">
+        <v>15.756</v>
+      </c>
+      <c r="C31" s="4">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>3.3199999998323619</v>
+      </c>
+      <c r="B32" s="4">
+        <v>15.949</v>
+      </c>
+      <c r="C32" s="4">
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>3.572999999858439</v>
+      </c>
+      <c r="B33" s="4">
+        <v>16.023</v>
+      </c>
+      <c r="C33" s="4">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>3.5740000000223522</v>
+      </c>
+      <c r="B34" s="4">
+        <v>16.044</v>
+      </c>
+      <c r="C34" s="4">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>3.6669999998994172</v>
+      </c>
+      <c r="B35" s="4">
+        <v>16.059000000000001</v>
+      </c>
+      <c r="C35" s="4">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>3.6680000000633299</v>
+      </c>
+      <c r="B36" s="4">
+        <v>16.085000000000001</v>
+      </c>
+      <c r="C36" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>3.697999999858439</v>
+      </c>
+      <c r="B37" s="4">
+        <v>16.114999999999998</v>
+      </c>
+      <c r="C37" s="4">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>3.6990000000223522</v>
+      </c>
+      <c r="B38" s="4">
+        <v>16.123000000000001</v>
+      </c>
+      <c r="C38" s="4">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>3.8739999998360868</v>
+      </c>
+      <c r="B39" s="4">
+        <v>16.207999999999998</v>
+      </c>
+      <c r="C39" s="4">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>3.875</v>
+      </c>
+      <c r="B40" s="4">
+        <v>16.187000000000001</v>
+      </c>
+      <c r="C40" s="4">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>3.8879999998025601</v>
+      </c>
+      <c r="B41" s="4">
+        <v>16.282</v>
+      </c>
+      <c r="C41" s="4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>3.8889999999664719</v>
+      </c>
+      <c r="B42" s="4">
+        <v>16.289000000000001</v>
+      </c>
+      <c r="C42" s="4">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="7"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="7"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="7"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="7"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="7"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="7"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEDE10A6-85AA-4949-9A9B-6500638E0C21}">
+  <dimension ref="A1:C121"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2832,7 +3533,7 @@
         <v>0.7361548</v>
       </c>
       <c r="B2" s="4">
-        <v>18.978000000000002</v>
+        <v>18.977</v>
       </c>
       <c r="C2" s="4">
         <v>0.08</v>
@@ -2843,7 +3544,7 @@
         <v>0.73452949000000001</v>
       </c>
       <c r="B3" s="4">
-        <v>19.058</v>
+        <v>19.056999999999999</v>
       </c>
       <c r="C3" s="4">
         <v>0.13</v>
@@ -2854,7 +3555,7 @@
         <v>0.73629635999999998</v>
       </c>
       <c r="B4" s="4">
-        <v>18.968</v>
+        <v>18.966999999999999</v>
       </c>
       <c r="C4" s="4">
         <v>0.13</v>
@@ -2865,7 +3566,7 @@
         <v>0.73793518000000002</v>
       </c>
       <c r="B5" s="4">
-        <v>18.928000000000001</v>
+        <v>18.927</v>
       </c>
       <c r="C5" s="4">
         <v>0.12</v>
@@ -2873,515 +3574,2566 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>0.74201744999999997</v>
+        <v>0.73376156999999997</v>
       </c>
       <c r="B6" s="4">
-        <v>18.768000000000001</v>
+        <v>18.896999999999998</v>
       </c>
       <c r="C6" s="4">
-        <v>7.0000000000000007E-2</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>0.73999994999999996</v>
+        <v>0.73410880000000001</v>
       </c>
       <c r="B7" s="4">
-        <v>18.698</v>
+        <v>19.497</v>
       </c>
       <c r="C7" s="4">
-        <v>0.12</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>0.74130099999999999</v>
+        <v>0.73439814999999997</v>
       </c>
       <c r="B8" s="4">
-        <v>18.698</v>
+        <v>18.896999999999998</v>
       </c>
       <c r="C8" s="4">
-        <v>0.08</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>0.74262035000000004</v>
+        <v>0.73468750000000005</v>
       </c>
       <c r="B9" s="4">
-        <v>18.738</v>
+        <v>18.716999999999999</v>
       </c>
       <c r="C9" s="4">
-        <v>0.1</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>0.74414860999999999</v>
+        <v>0.73496528000000005</v>
       </c>
       <c r="B10" s="4">
-        <v>18.738</v>
+        <v>19.596999999999998</v>
       </c>
       <c r="C10" s="4">
-        <v>0.15</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>0.74817347000000001</v>
+        <v>0.73525463000000002</v>
       </c>
       <c r="B11" s="4">
-        <v>18.428000000000001</v>
+        <v>19.356999999999999</v>
       </c>
       <c r="C11" s="4">
-        <v>0.05</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>0.74595498999999998</v>
+        <v>0.73554397999999999</v>
       </c>
       <c r="B12" s="4">
-        <v>18.408000000000001</v>
+        <v>18.957000000000001</v>
       </c>
       <c r="C12" s="4">
-        <v>0.08</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>0.74763661999999997</v>
+        <v>0.73585648000000003</v>
       </c>
       <c r="B13" s="4">
-        <v>18.548000000000002</v>
+        <v>19.207000000000001</v>
       </c>
       <c r="C13" s="4">
-        <v>0.09</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>0.74904883</v>
+        <v>0.73614583</v>
       </c>
       <c r="B14" s="4">
-        <v>18.498000000000001</v>
+        <v>19.087</v>
       </c>
       <c r="C14" s="4">
-        <v>0.09</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
-        <v>0.75049745999999995</v>
-      </c>
-      <c r="B15" s="6">
-        <v>18.288</v>
-      </c>
-      <c r="C15" s="6">
-        <v>0.08</v>
+      <c r="A15" s="4">
+        <v>0.73644675999999998</v>
+      </c>
+      <c r="B15" s="4">
+        <v>18.396999999999998</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.12</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>1.799000000115484</v>
+        <v>0.73673611000000006</v>
       </c>
       <c r="B16" s="4">
-        <v>14.672000000000001</v>
+        <v>19.346999999999998</v>
       </c>
       <c r="C16" s="4">
-        <v>0.04</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>1.799000000115484</v>
+        <v>0.73704860999999999</v>
       </c>
       <c r="B17" s="4">
-        <v>14.672000000000001</v>
+        <v>19.536999999999999</v>
       </c>
       <c r="C17" s="4">
-        <v>0.04</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>2.1650000000372529</v>
+        <v>0.73734953999999997</v>
       </c>
       <c r="B18" s="4">
-        <v>14.789</v>
+        <v>19.117000000000001</v>
       </c>
       <c r="C18" s="4">
-        <v>6.4000000000000001E-2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>2.2310000001452859</v>
+        <v>0.73765046000000001</v>
       </c>
       <c r="B19" s="4">
-        <v>14.957000000000001</v>
+        <v>19.177</v>
       </c>
       <c r="C19" s="4">
-        <v>6.0999999999999999E-2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>2.6069999998435378</v>
+        <v>0.73793982000000002</v>
       </c>
       <c r="B20" s="4">
-        <v>15.106</v>
+        <v>18.617000000000001</v>
       </c>
       <c r="C20" s="4">
-        <v>1.2E-2</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>2.608000000007451</v>
+        <v>0.73822916999999999</v>
       </c>
       <c r="B21" s="4">
-        <v>15.102</v>
+        <v>18.966999999999999</v>
       </c>
       <c r="C21" s="4">
-        <v>8.0000000000000002E-3</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>2.6290000001899898</v>
+        <v>0.73850693999999995</v>
       </c>
       <c r="B22" s="4">
-        <v>15.202</v>
+        <v>18.846999999999998</v>
       </c>
       <c r="C22" s="4">
-        <v>0.03</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <v>2.6290000001899898</v>
+        <v>0.74201744999999997</v>
       </c>
       <c r="B23" s="4">
-        <v>15.202</v>
+        <v>18.766999999999999</v>
       </c>
       <c r="C23" s="4">
-        <v>0.03</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <v>2.7880000001750891</v>
+        <v>0.73999994999999996</v>
       </c>
       <c r="B24" s="4">
-        <v>15.391999999999999</v>
+        <v>18.696999999999999</v>
       </c>
       <c r="C24" s="4">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <v>2.7880000001750891</v>
+        <v>0.74130099999999999</v>
       </c>
       <c r="B25" s="4">
-        <v>15.391999999999999</v>
+        <v>18.696999999999999</v>
       </c>
       <c r="C25" s="4">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <v>2.8209999999962752</v>
+        <v>0.74262035000000004</v>
       </c>
       <c r="B26" s="4">
-        <v>15.273999999999999</v>
+        <v>18.736999999999998</v>
       </c>
       <c r="C26" s="4">
-        <v>1.2E-2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
-        <v>2.822000000160187</v>
+        <v>0.74414860999999999</v>
       </c>
       <c r="B27" s="4">
-        <v>15.247</v>
+        <v>18.736999999999998</v>
       </c>
       <c r="C27" s="4">
-        <v>1.4E-2</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
-        <v>2.8960000001825388</v>
+        <v>0.73947916999999996</v>
       </c>
       <c r="B28" s="4">
-        <v>15.502000000000001</v>
+        <v>18.536999999999999</v>
       </c>
       <c r="C28" s="4">
-        <v>0.06</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <v>2.8960000001825388</v>
+        <v>0.73974536999999996</v>
       </c>
       <c r="B29" s="4">
-        <v>15.502000000000001</v>
+        <v>18.876999999999999</v>
       </c>
       <c r="C29" s="4">
-        <v>0.06</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <v>3.2349999998696148</v>
+        <v>0.74</v>
       </c>
       <c r="B30" s="4">
-        <v>15.651999999999999</v>
+        <v>18.766999999999999</v>
       </c>
       <c r="C30" s="4">
-        <v>7.4999999999999997E-2</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <v>3.31900000013411</v>
+        <v>0.74025463000000002</v>
       </c>
       <c r="B31" s="4">
-        <v>15.756</v>
+        <v>19.146999999999998</v>
       </c>
       <c r="C31" s="4">
-        <v>3.7999999999999999E-2</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <v>3.3199999998323619</v>
+        <v>0.74052083000000002</v>
       </c>
       <c r="B32" s="4">
-        <v>15.949</v>
+        <v>18.477</v>
       </c>
       <c r="C32" s="4">
-        <v>3.4000000000000002E-2</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
-        <v>3.572999999858439</v>
+        <v>0.74077546000000005</v>
       </c>
       <c r="B33" s="4">
-        <v>16.023</v>
+        <v>18.997</v>
       </c>
       <c r="C33" s="4">
-        <v>1.6E-2</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <v>3.5740000000223522</v>
+        <v>0.74104166999999999</v>
       </c>
       <c r="B34" s="4">
-        <v>16.044</v>
+        <v>18.297000000000001</v>
       </c>
       <c r="C34" s="4">
-        <v>1.7999999999999999E-2</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
-        <v>3.6669999998994172</v>
+        <v>0.74129630000000002</v>
       </c>
       <c r="B35" s="4">
-        <v>16.059000000000001</v>
+        <v>18.957000000000001</v>
       </c>
       <c r="C35" s="4">
-        <v>2.1000000000000001E-2</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
-        <v>3.6680000000633299</v>
+        <v>0.74156250000000001</v>
       </c>
       <c r="B36" s="4">
-        <v>16.085000000000001</v>
+        <v>18.466999999999999</v>
       </c>
       <c r="C36" s="4">
-        <v>0.02</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
-        <v>3.697999999858439</v>
+        <v>0.74182870000000001</v>
       </c>
       <c r="B37" s="4">
-        <v>16.114999999999998</v>
+        <v>18.986999999999998</v>
       </c>
       <c r="C37" s="4">
-        <v>2.3E-2</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <v>3.6990000000223522</v>
+        <v>0.74208333000000004</v>
       </c>
       <c r="B38" s="4">
-        <v>16.123000000000001</v>
+        <v>18.407</v>
       </c>
       <c r="C38" s="4">
-        <v>1.7999999999999999E-2</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
-        <v>3.8739999998360868</v>
+        <v>0.74234953999999997</v>
       </c>
       <c r="B39" s="4">
-        <v>16.207999999999998</v>
+        <v>19.826999999999998</v>
       </c>
       <c r="C39" s="4">
-        <v>2.1000000000000001E-2</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
-        <v>3.875</v>
+        <v>0.74261573999999997</v>
       </c>
       <c r="B40" s="4">
-        <v>16.187000000000001</v>
+        <v>19.266999999999999</v>
       </c>
       <c r="C40" s="4">
-        <v>2.1999999999999999E-2</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
-        <v>3.8879999998025601</v>
+        <v>0.74287037</v>
       </c>
       <c r="B41" s="4">
-        <v>16.282</v>
+        <v>18.657</v>
       </c>
       <c r="C41" s="4">
-        <v>1.4999999999999999E-2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
+        <v>0.74318287000000005</v>
+      </c>
+      <c r="B42" s="4">
+        <v>18.776999999999997</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>0.74351851999999996</v>
+      </c>
+      <c r="B43" s="4">
+        <v>18.887</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>0.74384258999999997</v>
+      </c>
+      <c r="B44" s="4">
+        <v>18.957000000000001</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>0.74414351999999995</v>
+      </c>
+      <c r="B45" s="4">
+        <v>18.986999999999998</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>0.74446758999999996</v>
+      </c>
+      <c r="B46" s="4">
+        <v>18.576999999999998</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>0.74476852000000004</v>
+      </c>
+      <c r="B47" s="4">
+        <v>18.526999999999997</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>0.74817347000000001</v>
+      </c>
+      <c r="B48" s="4">
+        <v>18.427</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>0.74595498999999998</v>
+      </c>
+      <c r="B49" s="4">
+        <v>18.407</v>
+      </c>
+      <c r="C49" s="4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>0.74763661999999997</v>
+      </c>
+      <c r="B50" s="4">
+        <v>18.547000000000001</v>
+      </c>
+      <c r="C50" s="4">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>0.74904883</v>
+      </c>
+      <c r="B51" s="4">
+        <v>18.497</v>
+      </c>
+      <c r="C51" s="4">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>0.75049745999999995</v>
+      </c>
+      <c r="B52" s="4">
+        <v>18.286999999999999</v>
+      </c>
+      <c r="C52" s="4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>0.74512730999999999</v>
+      </c>
+      <c r="B53" s="4">
+        <v>18.646999999999998</v>
+      </c>
+      <c r="C53" s="4">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>0.74550925999999995</v>
+      </c>
+      <c r="B54" s="4">
+        <v>18.337</v>
+      </c>
+      <c r="C54" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>0.74582176</v>
+      </c>
+      <c r="B55" s="4">
+        <v>18.747</v>
+      </c>
+      <c r="C55" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>0.74612268999999998</v>
+      </c>
+      <c r="B56" s="4">
+        <v>18.707000000000001</v>
+      </c>
+      <c r="C56" s="4">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>0.74642361000000002</v>
+      </c>
+      <c r="B57" s="4">
+        <v>18.056999999999999</v>
+      </c>
+      <c r="C57" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>0.74672453999999999</v>
+      </c>
+      <c r="B58" s="4">
+        <v>18.416999999999998</v>
+      </c>
+      <c r="C58" s="4">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>0.74706019000000001</v>
+      </c>
+      <c r="B59" s="4">
+        <v>18.376999999999999</v>
+      </c>
+      <c r="C59" s="4">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <v>0.74737268999999995</v>
+      </c>
+      <c r="B60" s="4">
+        <v>18.617000000000001</v>
+      </c>
+      <c r="C60" s="4">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
+        <v>0.74765046000000002</v>
+      </c>
+      <c r="B61" s="4">
+        <v>18.786999999999999</v>
+      </c>
+      <c r="C61" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
+        <v>0.74791666999999995</v>
+      </c>
+      <c r="B62" s="4">
+        <v>18.497</v>
+      </c>
+      <c r="C62" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="4">
+        <v>0.74818287000000006</v>
+      </c>
+      <c r="B63" s="4">
+        <v>18.376999999999999</v>
+      </c>
+      <c r="C63" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="4">
+        <v>0.74843749999999998</v>
+      </c>
+      <c r="B64" s="4">
+        <v>18.576999999999998</v>
+      </c>
+      <c r="C64" s="4">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="4">
+        <v>0.74870369999999997</v>
+      </c>
+      <c r="B65" s="4">
+        <v>18.297000000000001</v>
+      </c>
+      <c r="C65" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
+        <v>0.74906249999999996</v>
+      </c>
+      <c r="B66" s="4">
+        <v>18.567</v>
+      </c>
+      <c r="C66" s="4">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="4">
+        <v>0.74938656999999997</v>
+      </c>
+      <c r="B67" s="4">
+        <v>18.137</v>
+      </c>
+      <c r="C67" s="4">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
+        <v>0.74965278000000002</v>
+      </c>
+      <c r="B68" s="4">
+        <v>19.117000000000001</v>
+      </c>
+      <c r="C68" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
+        <v>0.74994212999999998</v>
+      </c>
+      <c r="B69" s="4">
+        <v>18.256999999999998</v>
+      </c>
+      <c r="C69" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
+        <v>0.75023147999999995</v>
+      </c>
+      <c r="B70" s="4">
+        <v>18.376999999999999</v>
+      </c>
+      <c r="C70" s="4">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="4">
+        <v>0.75050925999999996</v>
+      </c>
+      <c r="B71" s="4">
+        <v>18.177</v>
+      </c>
+      <c r="C71" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="4">
+        <v>0.75077545999999995</v>
+      </c>
+      <c r="B72" s="4">
+        <v>18.457000000000001</v>
+      </c>
+      <c r="C72" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="5">
+        <v>0.75103008999999998</v>
+      </c>
+      <c r="B73" s="5">
+        <v>18.266999999999999</v>
+      </c>
+      <c r="C73" s="5">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>1.799000000115484</v>
+      </c>
+      <c r="B74" s="4">
+        <v>14.672000000000001</v>
+      </c>
+      <c r="C74" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
+        <v>1.799000000115484</v>
+      </c>
+      <c r="B75" s="4">
+        <v>14.672000000000001</v>
+      </c>
+      <c r="C75" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
+        <v>2.1650000000372529</v>
+      </c>
+      <c r="B76" s="4">
+        <v>14.789</v>
+      </c>
+      <c r="C76" s="4">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="4">
+        <v>2.2310000001452859</v>
+      </c>
+      <c r="B77" s="4">
+        <v>14.957000000000001</v>
+      </c>
+      <c r="C77" s="4">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="4">
+        <v>2.6069999998435378</v>
+      </c>
+      <c r="B78" s="4">
+        <v>15.106</v>
+      </c>
+      <c r="C78" s="4">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="4">
+        <v>2.608000000007451</v>
+      </c>
+      <c r="B79" s="4">
+        <v>15.102</v>
+      </c>
+      <c r="C79" s="4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="4">
+        <v>2.6290000001899898</v>
+      </c>
+      <c r="B80" s="4">
+        <v>15.202</v>
+      </c>
+      <c r="C80" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="4">
+        <v>2.6290000001899898</v>
+      </c>
+      <c r="B81" s="4">
+        <v>15.202</v>
+      </c>
+      <c r="C81" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="4">
+        <v>2.7880000001750891</v>
+      </c>
+      <c r="B82" s="4">
+        <v>15.391999999999999</v>
+      </c>
+      <c r="C82" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="4">
+        <v>2.7880000001750891</v>
+      </c>
+      <c r="B83" s="4">
+        <v>15.391999999999999</v>
+      </c>
+      <c r="C83" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="4">
+        <v>2.8209999999962752</v>
+      </c>
+      <c r="B84" s="4">
+        <v>15.273999999999999</v>
+      </c>
+      <c r="C84" s="4">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
+        <v>2.822000000160187</v>
+      </c>
+      <c r="B85" s="4">
+        <v>15.247</v>
+      </c>
+      <c r="C85" s="4">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="4">
+        <v>2.8960000001825388</v>
+      </c>
+      <c r="B86" s="4">
+        <v>15.502000000000001</v>
+      </c>
+      <c r="C86" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="4">
+        <v>2.8960000001825388</v>
+      </c>
+      <c r="B87" s="4">
+        <v>15.502000000000001</v>
+      </c>
+      <c r="C87" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="4">
+        <v>3.2349999998696148</v>
+      </c>
+      <c r="B88" s="4">
+        <v>15.651999999999999</v>
+      </c>
+      <c r="C88" s="4">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="4">
+        <v>3.31900000013411</v>
+      </c>
+      <c r="B89" s="4">
+        <v>15.756</v>
+      </c>
+      <c r="C89" s="4">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="4">
+        <v>3.3199999998323619</v>
+      </c>
+      <c r="B90" s="4">
+        <v>15.949</v>
+      </c>
+      <c r="C90" s="4">
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="4">
+        <v>3.572999999858439</v>
+      </c>
+      <c r="B91" s="4">
+        <v>16.023</v>
+      </c>
+      <c r="C91" s="4">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="4">
+        <v>3.5740000000223522</v>
+      </c>
+      <c r="B92" s="4">
+        <v>16.044</v>
+      </c>
+      <c r="C92" s="4">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="4">
+        <v>3.6669999998994172</v>
+      </c>
+      <c r="B93" s="4">
+        <v>16.059000000000001</v>
+      </c>
+      <c r="C93" s="4">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="4">
+        <v>3.6680000000633299</v>
+      </c>
+      <c r="B94" s="4">
+        <v>16.085000000000001</v>
+      </c>
+      <c r="C94" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="4">
+        <v>3.697999999858439</v>
+      </c>
+      <c r="B95" s="4">
+        <v>16.114999999999998</v>
+      </c>
+      <c r="C95" s="4">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="4">
+        <v>3.6990000000223522</v>
+      </c>
+      <c r="B96" s="4">
+        <v>16.123000000000001</v>
+      </c>
+      <c r="C96" s="4">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="4">
+        <v>3.8739999998360868</v>
+      </c>
+      <c r="B97" s="4">
+        <v>16.207999999999998</v>
+      </c>
+      <c r="C97" s="4">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="4">
+        <v>3.875</v>
+      </c>
+      <c r="B98" s="4">
+        <v>16.187000000000001</v>
+      </c>
+      <c r="C98" s="4">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="4">
+        <v>3.8879999998025601</v>
+      </c>
+      <c r="B99" s="4">
+        <v>16.282</v>
+      </c>
+      <c r="C99" s="4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="4">
         <v>3.8889999999664719</v>
       </c>
+      <c r="B100" s="4">
+        <v>16.289000000000001</v>
+      </c>
+      <c r="C100" s="4">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="4"/>
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="4"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="4"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="4"/>
+      <c r="B104" s="4"/>
+      <c r="C104" s="4"/>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="4"/>
+      <c r="B105" s="4"/>
+      <c r="C105" s="4"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="4"/>
+      <c r="B106" s="4"/>
+      <c r="C106" s="4"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="4"/>
+      <c r="B107" s="4"/>
+      <c r="C107" s="4"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="4"/>
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="4"/>
+      <c r="B109" s="4"/>
+      <c r="C109" s="4"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="4"/>
+      <c r="B110" s="4"/>
+      <c r="C110" s="4"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="4"/>
+      <c r="B111" s="4"/>
+      <c r="C111" s="4"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="4"/>
+      <c r="B112" s="4"/>
+      <c r="C112" s="4"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="4"/>
+      <c r="B113" s="4"/>
+      <c r="C113" s="4"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="4"/>
+      <c r="B114" s="4"/>
+      <c r="C114" s="4"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="4"/>
+      <c r="B115" s="4"/>
+      <c r="C115" s="4"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="4"/>
+      <c r="B116" s="4"/>
+      <c r="C116" s="4"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="4"/>
+      <c r="B117" s="4"/>
+      <c r="C117" s="4"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="4"/>
+      <c r="B118" s="4"/>
+      <c r="C118" s="4"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="4"/>
+      <c r="B119" s="4"/>
+      <c r="C119" s="4"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="4"/>
+      <c r="B120" s="4"/>
+      <c r="C120" s="4"/>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="4"/>
+      <c r="B121" s="4"/>
+      <c r="C121" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932FF3B4-025A-4C2A-8070-653345A7B6BC}">
+  <dimension ref="A1:C127"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>0.7361548</v>
+      </c>
+      <c r="B2" s="4">
+        <v>18.977</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>0.73452949000000001</v>
+      </c>
+      <c r="B3" s="4">
+        <v>19.056999999999999</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>0.73629635999999998</v>
+      </c>
+      <c r="B4" s="4">
+        <v>18.966999999999999</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>0.73793518000000002</v>
+      </c>
+      <c r="B5" s="4">
+        <v>18.927</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>0.73376156999999997</v>
+      </c>
+      <c r="B6" s="4">
+        <v>18.896999999999998</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>0.73410880000000001</v>
+      </c>
+      <c r="B7" s="4">
+        <v>19.497</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>0.73439814999999997</v>
+      </c>
+      <c r="B8" s="4">
+        <v>18.896999999999998</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>0.73468750000000005</v>
+      </c>
+      <c r="B9" s="4">
+        <v>18.716999999999999</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>0.73496528000000005</v>
+      </c>
+      <c r="B10" s="4">
+        <v>19.596999999999998</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>0.73525463000000002</v>
+      </c>
+      <c r="B11" s="4">
+        <v>19.356999999999999</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>0.73554397999999999</v>
+      </c>
+      <c r="B12" s="4">
+        <v>18.957000000000001</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>0.73585648000000003</v>
+      </c>
+      <c r="B13" s="4">
+        <v>19.207000000000001</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>0.73614583</v>
+      </c>
+      <c r="B14" s="4">
+        <v>19.087</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>0.73644675999999998</v>
+      </c>
+      <c r="B15" s="4">
+        <v>18.396999999999998</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>0.73673611000000006</v>
+      </c>
+      <c r="B16" s="4">
+        <v>19.346999999999998</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>0.73704860999999999</v>
+      </c>
+      <c r="B17" s="4">
+        <v>19.536999999999999</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>0.73734953999999997</v>
+      </c>
+      <c r="B18" s="4">
+        <v>19.117000000000001</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>0.73765046000000001</v>
+      </c>
+      <c r="B19" s="4">
+        <v>19.177</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>0.73793982000000002</v>
+      </c>
+      <c r="B20" s="4">
+        <v>18.617000000000001</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>0.73822916999999999</v>
+      </c>
+      <c r="B21" s="4">
+        <v>18.966999999999999</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>0.73850693999999995</v>
+      </c>
+      <c r="B22" s="4">
+        <v>18.846999999999998</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>0.74201744999999997</v>
+      </c>
+      <c r="B23" s="4">
+        <v>18.766999999999999</v>
+      </c>
+      <c r="C23" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>0.73999994999999996</v>
+      </c>
+      <c r="B24" s="4">
+        <v>18.696999999999999</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>0.74130099999999999</v>
+      </c>
+      <c r="B25" s="4">
+        <v>18.696999999999999</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>0.74262035000000004</v>
+      </c>
+      <c r="B26" s="4">
+        <v>18.736999999999998</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>0.74414860999999999</v>
+      </c>
+      <c r="B27" s="4">
+        <v>18.736999999999998</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>0.73947916999999996</v>
+      </c>
+      <c r="B28" s="4">
+        <v>18.536999999999999</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>0.73974536999999996</v>
+      </c>
+      <c r="B29" s="4">
+        <v>18.876999999999999</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>0.74</v>
+      </c>
+      <c r="B30" s="4">
+        <v>18.766999999999999</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>0.74025463000000002</v>
+      </c>
+      <c r="B31" s="4">
+        <v>19.146999999999998</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>0.74052083000000002</v>
+      </c>
+      <c r="B32" s="4">
+        <v>18.477</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>0.74077546000000005</v>
+      </c>
+      <c r="B33" s="4">
+        <v>18.997</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>0.74104166999999999</v>
+      </c>
+      <c r="B34" s="4">
+        <v>18.297000000000001</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>0.74129630000000002</v>
+      </c>
+      <c r="B35" s="4">
+        <v>18.957000000000001</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>0.74156250000000001</v>
+      </c>
+      <c r="B36" s="4">
+        <v>18.466999999999999</v>
+      </c>
+      <c r="C36" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>0.74182870000000001</v>
+      </c>
+      <c r="B37" s="4">
+        <v>18.986999999999998</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>0.74208333000000004</v>
+      </c>
+      <c r="B38" s="4">
+        <v>18.407</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>0.74234953999999997</v>
+      </c>
+      <c r="B39" s="4">
+        <v>19.826999999999998</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>0.74261573999999997</v>
+      </c>
+      <c r="B40" s="4">
+        <v>19.266999999999999</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>0.74287037</v>
+      </c>
+      <c r="B41" s="4">
+        <v>18.657</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>0.74318287000000005</v>
+      </c>
       <c r="B42" s="4">
+        <v>18.776999999999997</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>0.74351851999999996</v>
+      </c>
+      <c r="B43" s="4">
+        <v>18.887</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>0.74384258999999997</v>
+      </c>
+      <c r="B44" s="4">
+        <v>18.957000000000001</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>0.74414351999999995</v>
+      </c>
+      <c r="B45" s="4">
+        <v>18.986999999999998</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>0.74446758999999996</v>
+      </c>
+      <c r="B46" s="4">
+        <v>18.576999999999998</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>0.74476852000000004</v>
+      </c>
+      <c r="B47" s="4">
+        <v>18.526999999999997</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>0.74817347000000001</v>
+      </c>
+      <c r="B48" s="4">
+        <v>18.427</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>0.74595498999999998</v>
+      </c>
+      <c r="B49" s="4">
+        <v>18.407</v>
+      </c>
+      <c r="C49" s="4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>0.74763661999999997</v>
+      </c>
+      <c r="B50" s="4">
+        <v>18.547000000000001</v>
+      </c>
+      <c r="C50" s="4">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>0.74904883</v>
+      </c>
+      <c r="B51" s="4">
+        <v>18.497</v>
+      </c>
+      <c r="C51" s="4">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>0.75049745999999995</v>
+      </c>
+      <c r="B52" s="4">
+        <v>18.286999999999999</v>
+      </c>
+      <c r="C52" s="4">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>0.74512730999999999</v>
+      </c>
+      <c r="B53" s="4">
+        <v>18.646999999999998</v>
+      </c>
+      <c r="C53" s="4">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>0.74550925999999995</v>
+      </c>
+      <c r="B54" s="4">
+        <v>18.337</v>
+      </c>
+      <c r="C54" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>0.74582176</v>
+      </c>
+      <c r="B55" s="4">
+        <v>18.747</v>
+      </c>
+      <c r="C55" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>0.74612268999999998</v>
+      </c>
+      <c r="B56" s="4">
+        <v>18.707000000000001</v>
+      </c>
+      <c r="C56" s="4">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>0.74642361000000002</v>
+      </c>
+      <c r="B57" s="4">
+        <v>18.056999999999999</v>
+      </c>
+      <c r="C57" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>0.74672453999999999</v>
+      </c>
+      <c r="B58" s="4">
+        <v>18.416999999999998</v>
+      </c>
+      <c r="C58" s="4">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>0.74706019000000001</v>
+      </c>
+      <c r="B59" s="4">
+        <v>18.376999999999999</v>
+      </c>
+      <c r="C59" s="4">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <v>0.74737268999999995</v>
+      </c>
+      <c r="B60" s="4">
+        <v>18.617000000000001</v>
+      </c>
+      <c r="C60" s="4">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
+        <v>0.74765046000000002</v>
+      </c>
+      <c r="B61" s="4">
+        <v>18.786999999999999</v>
+      </c>
+      <c r="C61" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
+        <v>0.74791666999999995</v>
+      </c>
+      <c r="B62" s="4">
+        <v>18.497</v>
+      </c>
+      <c r="C62" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="4">
+        <v>0.74818287000000006</v>
+      </c>
+      <c r="B63" s="4">
+        <v>18.376999999999999</v>
+      </c>
+      <c r="C63" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="4">
+        <v>0.74843749999999998</v>
+      </c>
+      <c r="B64" s="4">
+        <v>18.576999999999998</v>
+      </c>
+      <c r="C64" s="4">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="4">
+        <v>0.74870369999999997</v>
+      </c>
+      <c r="B65" s="4">
+        <v>18.297000000000001</v>
+      </c>
+      <c r="C65" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
+        <v>0.74906249999999996</v>
+      </c>
+      <c r="B66" s="4">
+        <v>18.567</v>
+      </c>
+      <c r="C66" s="4">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="4">
+        <v>0.74938656999999997</v>
+      </c>
+      <c r="B67" s="4">
+        <v>18.137</v>
+      </c>
+      <c r="C67" s="4">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
+        <v>0.74965278000000002</v>
+      </c>
+      <c r="B68" s="4">
+        <v>19.117000000000001</v>
+      </c>
+      <c r="C68" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
+        <v>0.74994212999999998</v>
+      </c>
+      <c r="B69" s="4">
+        <v>18.256999999999998</v>
+      </c>
+      <c r="C69" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
+        <v>0.75023147999999995</v>
+      </c>
+      <c r="B70" s="4">
+        <v>18.376999999999999</v>
+      </c>
+      <c r="C70" s="4">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="4">
+        <v>0.75050925999999996</v>
+      </c>
+      <c r="B71" s="4">
+        <v>18.177</v>
+      </c>
+      <c r="C71" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="4">
+        <v>0.75077545999999995</v>
+      </c>
+      <c r="B72" s="4">
+        <v>18.457000000000001</v>
+      </c>
+      <c r="C72" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="5">
+        <v>0.75103008999999998</v>
+      </c>
+      <c r="B73" s="5">
+        <v>18.266999999999999</v>
+      </c>
+      <c r="C73" s="5">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>1.799000000115484</v>
+      </c>
+      <c r="B74" s="4">
+        <v>14.672000000000001</v>
+      </c>
+      <c r="C74" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
+        <v>1.799000000115484</v>
+      </c>
+      <c r="B75" s="4">
+        <v>14.672000000000001</v>
+      </c>
+      <c r="C75" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
+        <v>2.1650000000372529</v>
+      </c>
+      <c r="B76" s="4">
+        <v>14.789</v>
+      </c>
+      <c r="C76" s="4">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="4">
+        <v>2.2310000001452859</v>
+      </c>
+      <c r="B77" s="4">
+        <v>14.957000000000001</v>
+      </c>
+      <c r="C77" s="4">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="4">
+        <v>2.6069999998435378</v>
+      </c>
+      <c r="B78" s="4">
+        <v>15.106</v>
+      </c>
+      <c r="C78" s="4">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="4">
+        <v>2.608000000007451</v>
+      </c>
+      <c r="B79" s="4">
+        <v>15.102</v>
+      </c>
+      <c r="C79" s="4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="4">
+        <v>2.6290000001899898</v>
+      </c>
+      <c r="B80" s="4">
+        <v>15.202</v>
+      </c>
+      <c r="C80" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="4">
+        <v>2.6290000001899898</v>
+      </c>
+      <c r="B81" s="4">
+        <v>15.202</v>
+      </c>
+      <c r="C81" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="4">
+        <v>2.7880000001750891</v>
+      </c>
+      <c r="B82" s="4">
+        <v>15.391999999999999</v>
+      </c>
+      <c r="C82" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="4">
+        <v>2.7880000001750891</v>
+      </c>
+      <c r="B83" s="4">
+        <v>15.391999999999999</v>
+      </c>
+      <c r="C83" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="4">
+        <v>2.8209999999962752</v>
+      </c>
+      <c r="B84" s="4">
+        <v>15.273999999999999</v>
+      </c>
+      <c r="C84" s="4">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
+        <v>2.822000000160187</v>
+      </c>
+      <c r="B85" s="4">
+        <v>15.247</v>
+      </c>
+      <c r="C85" s="4">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="4">
+        <v>2.8960000001825388</v>
+      </c>
+      <c r="B86" s="4">
+        <v>15.502000000000001</v>
+      </c>
+      <c r="C86" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="4">
+        <v>2.8960000001825388</v>
+      </c>
+      <c r="B87" s="4">
+        <v>15.502000000000001</v>
+      </c>
+      <c r="C87" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="4">
+        <v>3.2349999998696148</v>
+      </c>
+      <c r="B88" s="4">
+        <v>15.651999999999999</v>
+      </c>
+      <c r="C88" s="4">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="4">
+        <v>3.31900000013411</v>
+      </c>
+      <c r="B89" s="4">
+        <v>15.756</v>
+      </c>
+      <c r="C89" s="4">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="4">
+        <v>3.3199999998323619</v>
+      </c>
+      <c r="B90" s="4">
+        <v>15.949</v>
+      </c>
+      <c r="C90" s="4">
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="4">
+        <v>3.572999999858439</v>
+      </c>
+      <c r="B91" s="4">
+        <v>16.023</v>
+      </c>
+      <c r="C91" s="4">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="4">
+        <v>3.5740000000223522</v>
+      </c>
+      <c r="B92" s="4">
+        <v>16.044</v>
+      </c>
+      <c r="C92" s="4">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="4">
+        <v>3.6669999998994172</v>
+      </c>
+      <c r="B93" s="4">
+        <v>16.059000000000001</v>
+      </c>
+      <c r="C93" s="4">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="4">
+        <v>3.6680000000633299</v>
+      </c>
+      <c r="B94" s="4">
+        <v>16.085000000000001</v>
+      </c>
+      <c r="C94" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="4">
+        <v>3.697999999858439</v>
+      </c>
+      <c r="B95" s="4">
+        <v>16.114999999999998</v>
+      </c>
+      <c r="C95" s="4">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="4">
+        <v>3.6990000000223522</v>
+      </c>
+      <c r="B96" s="4">
+        <v>16.123000000000001</v>
+      </c>
+      <c r="C96" s="4">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="4">
+        <v>3.8739999998360868</v>
+      </c>
+      <c r="B97" s="4">
+        <v>16.207999999999998</v>
+      </c>
+      <c r="C97" s="4">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="4">
+        <v>3.875</v>
+      </c>
+      <c r="B98" s="4">
+        <v>16.187000000000001</v>
+      </c>
+      <c r="C98" s="4">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="4">
+        <v>3.8879999998025601</v>
+      </c>
+      <c r="B99" s="4">
+        <v>16.282</v>
+      </c>
+      <c r="C99" s="4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="4">
+        <v>3.8889999999664719</v>
+      </c>
+      <c r="B100" s="4">
         <v>16.289000000000001</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C100" s="4">
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="7"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="7"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
-      <c r="B59" s="7"/>
-      <c r="C59" s="7"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="7"/>
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="7"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="7"/>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="7"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="4">
+        <v>1.799000000115484</v>
+      </c>
+      <c r="B101" s="4">
+        <v>14.672000000000001</v>
+      </c>
+      <c r="C101" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="4">
+        <v>1.799000000115484</v>
+      </c>
+      <c r="B102" s="4">
+        <v>14.672000000000001</v>
+      </c>
+      <c r="C102" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="4">
+        <v>2.1650000000372529</v>
+      </c>
+      <c r="B103" s="4">
+        <v>14.789</v>
+      </c>
+      <c r="C103" s="4">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="4">
+        <v>2.2310000001452859</v>
+      </c>
+      <c r="B104" s="4">
+        <v>14.957000000000001</v>
+      </c>
+      <c r="C104" s="4">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="4">
+        <v>2.6069999998435378</v>
+      </c>
+      <c r="B105" s="4">
+        <v>15.106</v>
+      </c>
+      <c r="C105" s="4">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="4">
+        <v>2.608000000007451</v>
+      </c>
+      <c r="B106" s="4">
+        <v>15.102</v>
+      </c>
+      <c r="C106" s="4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="4">
+        <v>2.6290000001899898</v>
+      </c>
+      <c r="B107" s="4">
+        <v>15.202</v>
+      </c>
+      <c r="C107" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="4">
+        <v>2.6290000001899898</v>
+      </c>
+      <c r="B108" s="4">
+        <v>15.202</v>
+      </c>
+      <c r="C108" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="4">
+        <v>2.7880000001750891</v>
+      </c>
+      <c r="B109" s="4">
+        <v>15.391999999999999</v>
+      </c>
+      <c r="C109" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="4">
+        <v>2.7880000001750891</v>
+      </c>
+      <c r="B110" s="4">
+        <v>15.391999999999999</v>
+      </c>
+      <c r="C110" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="4">
+        <v>2.8209999999962752</v>
+      </c>
+      <c r="B111" s="4">
+        <v>15.273999999999999</v>
+      </c>
+      <c r="C111" s="4">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="4">
+        <v>2.822000000160187</v>
+      </c>
+      <c r="B112" s="4">
+        <v>15.247</v>
+      </c>
+      <c r="C112" s="4">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="4">
+        <v>2.8960000001825388</v>
+      </c>
+      <c r="B113" s="4">
+        <v>15.502000000000001</v>
+      </c>
+      <c r="C113" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="4">
+        <v>2.8960000001825388</v>
+      </c>
+      <c r="B114" s="4">
+        <v>15.502000000000001</v>
+      </c>
+      <c r="C114" s="4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="4">
+        <v>3.2349999998696148</v>
+      </c>
+      <c r="B115" s="4">
+        <v>15.651999999999999</v>
+      </c>
+      <c r="C115" s="4">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="4">
+        <v>3.31900000013411</v>
+      </c>
+      <c r="B116" s="4">
+        <v>15.756</v>
+      </c>
+      <c r="C116" s="4">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="4">
+        <v>3.3199999998323619</v>
+      </c>
+      <c r="B117" s="4">
+        <v>15.949</v>
+      </c>
+      <c r="C117" s="4">
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="4">
+        <v>3.572999999858439</v>
+      </c>
+      <c r="B118" s="4">
+        <v>16.023</v>
+      </c>
+      <c r="C118" s="4">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="4">
+        <v>3.5740000000223522</v>
+      </c>
+      <c r="B119" s="4">
+        <v>16.044</v>
+      </c>
+      <c r="C119" s="4">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="4">
+        <v>3.6669999998994172</v>
+      </c>
+      <c r="B120" s="4">
+        <v>16.059000000000001</v>
+      </c>
+      <c r="C120" s="4">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="4">
+        <v>3.6680000000633299</v>
+      </c>
+      <c r="B121" s="4">
+        <v>16.085000000000001</v>
+      </c>
+      <c r="C121" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="4">
+        <v>3.697999999858439</v>
+      </c>
+      <c r="B122" s="4">
+        <v>16.114999999999998</v>
+      </c>
+      <c r="C122" s="4">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="4">
+        <v>3.6990000000223522</v>
+      </c>
+      <c r="B123" s="4">
+        <v>16.123000000000001</v>
+      </c>
+      <c r="C123" s="4">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="4">
+        <v>3.8739999998360868</v>
+      </c>
+      <c r="B124" s="4">
+        <v>16.207999999999998</v>
+      </c>
+      <c r="C124" s="4">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="4">
+        <v>3.875</v>
+      </c>
+      <c r="B125" s="4">
+        <v>16.187000000000001</v>
+      </c>
+      <c r="C125" s="4">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="4">
+        <v>3.8879999998025601</v>
+      </c>
+      <c r="B126" s="4">
+        <v>16.282</v>
+      </c>
+      <c r="C126" s="4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="4">
+        <v>3.8889999999664719</v>
+      </c>
+      <c r="B127" s="4">
+        <v>16.289000000000001</v>
+      </c>
+      <c r="C127" s="4">
+        <v>1.4E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>